<commit_message>
Regression analysis: resAll fixed
</commit_message>
<xml_diff>
--- a/data/features.xlsx
+++ b/data/features.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="132">
   <si>
     <t>title</t>
   </si>
@@ -396,6 +396,33 @@
   </si>
   <si>
     <t>Redundant with genre</t>
+  </si>
+  <si>
+    <t>Redundant with box office success.</t>
+  </si>
+  <si>
+    <t>The studio that produced the film</t>
+  </si>
+  <si>
+    <t>Redundant with cast_votes_log</t>
+  </si>
+  <si>
+    <t>Redundant with director_experience_log</t>
+  </si>
+  <si>
+    <t>Redundant</t>
+  </si>
+  <si>
+    <t>Not in data set</t>
+  </si>
+  <si>
+    <t>Redundant with imdb_num_votes_log</t>
+  </si>
+  <si>
+    <t>Response variable</t>
+  </si>
+  <si>
+    <t>Redundant with cast_experience_log</t>
   </si>
 </sst>
 </file>
@@ -726,7 +753,7 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,6 +805,9 @@
       <c r="C2" t="s">
         <v>34</v>
       </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
       <c r="E2" t="s">
         <v>43</v>
       </c>
@@ -807,6 +837,9 @@
       <c r="C3" t="s">
         <v>34</v>
       </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
       <c r="E3" t="s">
         <v>43</v>
       </c>
@@ -836,6 +869,9 @@
       <c r="C4" t="s">
         <v>34</v>
       </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
@@ -865,6 +901,9 @@
       <c r="C5" t="s">
         <v>34</v>
       </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
       <c r="E5" t="s">
         <v>43</v>
       </c>
@@ -894,6 +933,9 @@
       <c r="C6" t="s">
         <v>34</v>
       </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
       <c r="E6" t="s">
         <v>43</v>
       </c>
@@ -923,6 +965,9 @@
       <c r="C7" t="s">
         <v>34</v>
       </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
       <c r="E7" t="s">
         <v>43</v>
       </c>
@@ -952,6 +997,9 @@
       <c r="C8" t="s">
         <v>34</v>
       </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
       <c r="E8" t="s">
         <v>43</v>
       </c>
@@ -981,6 +1029,9 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
       <c r="E9" t="s">
         <v>43</v>
       </c>
@@ -1010,6 +1061,9 @@
       <c r="C10" t="s">
         <v>34</v>
       </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
       <c r="E10" t="s">
         <v>43</v>
       </c>
@@ -1039,6 +1093,9 @@
       <c r="C11" t="s">
         <v>34</v>
       </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" t="s">
         <v>43</v>
       </c>
@@ -1068,6 +1125,9 @@
       <c r="C12" t="s">
         <v>34</v>
       </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
       <c r="E12" t="s">
         <v>43</v>
       </c>
@@ -1097,6 +1157,9 @@
       <c r="C13" t="s">
         <v>34</v>
       </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
       <c r="E13" t="s">
         <v>43</v>
       </c>
@@ -1126,6 +1189,9 @@
       <c r="C14" t="s">
         <v>34</v>
       </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
       <c r="E14" t="s">
         <v>43</v>
       </c>
@@ -1185,6 +1251,9 @@
         <v>34</v>
       </c>
       <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
         <v>34</v>
       </c>
       <c r="E16" t="s">
@@ -1221,7 +1290,7 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
         <v>43</v>
@@ -1254,7 +1323,7 @@
         <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
         <v>43</v>
@@ -1287,7 +1356,7 @@
         <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
         <v>43</v>
@@ -1320,7 +1389,7 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
         <v>43</v>
@@ -1353,7 +1422,7 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
         <v>43</v>
@@ -1385,6 +1454,9 @@
       <c r="C22" t="s">
         <v>33</v>
       </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
       <c r="E22" t="s">
         <v>43</v>
       </c>
@@ -1484,6 +1556,9 @@
       <c r="C25" t="s">
         <v>33</v>
       </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
       <c r="E25" t="s">
         <v>43</v>
       </c>
@@ -1500,6 +1575,9 @@
         <v>5</v>
       </c>
       <c r="J25" t="s">
+        <v>124</v>
+      </c>
+      <c r="K25" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1515,7 +1593,7 @@
         <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
         <v>43</v>
@@ -1568,7 +1646,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1603,13 +1681,13 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>A28+1</f>
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
         <v>33</v>
@@ -1635,8 +1713,11 @@
       <c r="J29" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>A29+1</f>
         <v>3</v>
@@ -1648,7 +1729,7 @@
         <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
         <v>43</v>
@@ -1680,6 +1761,9 @@
       <c r="C31" t="s">
         <v>34</v>
       </c>
+      <c r="D31" t="s">
+        <v>34</v>
+      </c>
       <c r="E31" t="s">
         <v>44</v>
       </c>
@@ -1697,6 +1781,9 @@
       </c>
       <c r="J31" t="s">
         <v>95</v>
+      </c>
+      <c r="K31" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1710,6 +1797,9 @@
       <c r="C32" t="s">
         <v>34</v>
       </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
       <c r="E32" t="s">
         <v>44</v>
       </c>
@@ -1728,8 +1818,11 @@
       <c r="J32" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>A30+1</f>
         <v>4</v>
@@ -1741,7 +1834,7 @@
         <v>33</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
         <v>44</v>
@@ -1761,8 +1854,11 @@
       <c r="J33" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>A32+1</f>
         <v>6</v>
@@ -1795,7 +1891,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>A34+1</f>
         <v>7</v>
@@ -1807,7 +1903,7 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
         <v>44</v>
@@ -1827,8 +1923,11 @@
       <c r="J35" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>A35+1</f>
         <v>8</v>
@@ -1861,7 +1960,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A36+1</f>
         <v>9</v>
@@ -1873,7 +1972,7 @@
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E37" t="s">
         <v>43</v>
@@ -1894,7 +1993,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>A36+1</f>
         <v>9</v>
@@ -1906,7 +2005,7 @@
         <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
         <v>44</v>
@@ -1926,8 +2025,11 @@
       <c r="J38" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>A37+1</f>
         <v>10</v>
@@ -1960,7 +2062,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>A37+1</f>
         <v>10</v>
@@ -1992,8 +2094,11 @@
       <c r="J40" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>A40+1</f>
         <v>11</v>
@@ -2005,7 +2110,7 @@
         <v>33</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E41" t="s">
         <v>44</v>
@@ -2025,8 +2130,11 @@
       <c r="J41" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>A41+1</f>
         <v>12</v>
@@ -2038,7 +2146,7 @@
         <v>33</v>
       </c>
       <c r="D42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E42" t="s">
         <v>43</v>
@@ -2059,7 +2167,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>A41+1</f>
         <v>12</v>
@@ -2070,6 +2178,9 @@
       <c r="C43" t="s">
         <v>34</v>
       </c>
+      <c r="D43" t="s">
+        <v>34</v>
+      </c>
       <c r="E43" t="s">
         <v>43</v>
       </c>
@@ -2088,8 +2199,11 @@
       <c r="J43" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>A42+1</f>
         <v>13</v>
@@ -2100,6 +2214,9 @@
       <c r="C44" t="s">
         <v>34</v>
       </c>
+      <c r="D44" t="s">
+        <v>33</v>
+      </c>
       <c r="E44" t="s">
         <v>44</v>
       </c>
@@ -2119,7 +2236,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <f>A44+1</f>
         <v>14</v>
@@ -2130,6 +2247,9 @@
       <c r="C45" t="s">
         <v>33</v>
       </c>
+      <c r="D45" t="s">
+        <v>33</v>
+      </c>
       <c r="E45" t="s">
         <v>44</v>
       </c>
@@ -2149,7 +2269,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <f>A45+1</f>
         <v>15</v>
@@ -2160,6 +2280,9 @@
       <c r="C46" t="s">
         <v>33</v>
       </c>
+      <c r="D46" t="s">
+        <v>34</v>
+      </c>
       <c r="E46" t="s">
         <v>44</v>
       </c>
@@ -2178,13 +2301,19 @@
       <c r="J46" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>33</v>
       </c>
       <c r="C47" t="s">
         <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>34</v>
       </c>
       <c r="E47" t="s">
         <v>44</v>
@@ -2204,12 +2333,18 @@
       <c r="J47" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>33</v>
       </c>
       <c r="C48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" t="s">
         <v>33</v>
       </c>
       <c r="E48" t="s">
@@ -2233,14 +2368,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K48">
-    <filterColumn colId="1">
+    <filterColumn colId="3">
       <filters>
         <filter val="yes"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Categorical"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added interpretation to regression analysis
</commit_message>
<xml_diff>
--- a/data/features.xlsx
+++ b/data/features.xlsx
@@ -15,7 +15,7 @@
     <sheet name="features" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">features!$A$1:$K$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">features!$A$1:$K$52</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="140">
   <si>
     <t>title</t>
   </si>
@@ -194,9 +194,6 @@
     <t>scores</t>
   </si>
   <si>
-    <t>10 * IMDB Rating + critics score + audience_score</t>
-  </si>
-  <si>
     <t>5. Performance</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
     <t>7. Box Office</t>
   </si>
   <si>
-    <t>box_office</t>
-  </si>
-  <si>
     <t>Title of movie</t>
   </si>
   <si>
@@ -308,21 +302,12 @@
     <t>Log number of IMDB votes</t>
   </si>
   <si>
-    <t>Total number of allocated IMDB votes for the cast of a film</t>
-  </si>
-  <si>
     <t>Total number of films in sample for a director</t>
   </si>
   <si>
-    <t>Box office revenue from BoxOfficeMojo.com</t>
-  </si>
-  <si>
     <t>imdb_num_votes_log</t>
   </si>
   <si>
-    <t>box_office_log</t>
-  </si>
-  <si>
     <t>Log of Box office revenue from BoxOfficeMojo.com</t>
   </si>
   <si>
@@ -335,24 +320,15 @@
     <t>cast_votes_log</t>
   </si>
   <si>
-    <t>Log of the total number of allocated IMDB votes for the cast of a film</t>
-  </si>
-  <si>
     <t>scores_log</t>
   </si>
   <si>
-    <t>Log(10 * IMDB Rating + critics score + audience_score)</t>
-  </si>
-  <si>
     <t>best_actress_win</t>
   </si>
   <si>
     <t>thtr_days</t>
   </si>
   <si>
-    <t>Number of days between theatre and dvd release</t>
-  </si>
-  <si>
     <t>director_experience_log</t>
   </si>
   <si>
@@ -374,9 +350,6 @@
     <t>thtr_days_log</t>
   </si>
   <si>
-    <t>Log number of days between theatre and dvd release</t>
-  </si>
-  <si>
     <t>Rationale</t>
   </si>
   <si>
@@ -386,43 +359,94 @@
     <t>Not predictive without other data</t>
   </si>
   <si>
-    <t>Redundant with critics_score</t>
-  </si>
-  <si>
-    <t>Redundant with audience_score</t>
-  </si>
-  <si>
-    <t>Not a variable that Paramount can change</t>
-  </si>
-  <si>
-    <t>Redundant with genre</t>
-  </si>
-  <si>
-    <t>Redundant with box office success.</t>
-  </si>
-  <si>
     <t>The studio that produced the film</t>
   </si>
   <si>
-    <t>Redundant with cast_votes_log</t>
-  </si>
-  <si>
-    <t>Redundant with director_experience_log</t>
-  </si>
-  <si>
-    <t>Redundant</t>
-  </si>
-  <si>
     <t>Not in data set</t>
   </si>
   <si>
-    <t>Redundant with imdb_num_votes_log</t>
-  </si>
-  <si>
-    <t>Response variable</t>
-  </si>
-  <si>
-    <t>Redundant with cast_experience_log</t>
+    <t>Average of 10 * IMDB Rating and audience_score</t>
+  </si>
+  <si>
+    <t>Log of thtr_days</t>
+  </si>
+  <si>
+    <t>votes_per_day</t>
+  </si>
+  <si>
+    <t>Log of scores</t>
+  </si>
+  <si>
+    <t>votes_per_day_log</t>
+  </si>
+  <si>
+    <t>Log of votes_per_day</t>
+  </si>
+  <si>
+    <t>daily_box_office</t>
+  </si>
+  <si>
+    <t>daily_box_office_log</t>
+  </si>
+  <si>
+    <t>Daily box office revenue from BoxOfficeMojo.com</t>
+  </si>
+  <si>
+    <t>Total number of allocated IMDB votes per day for the cast of a film</t>
+  </si>
+  <si>
+    <t>votes_per_day_scores</t>
+  </si>
+  <si>
+    <t>votes_per_day_scores_log</t>
+  </si>
+  <si>
+    <t>Highly correlated with cast_esperience_log</t>
+  </si>
+  <si>
+    <t>Highly correlated with cast_votes_log</t>
+  </si>
+  <si>
+    <t>Highly correlated with director_experience_log</t>
+  </si>
+  <si>
+    <t>Highly correlated with imdb_num_votes_log</t>
+  </si>
+  <si>
+    <t>Highly correlated with runtime_log</t>
+  </si>
+  <si>
+    <t>Highly correlated with votes_per_day_scores_log</t>
+  </si>
+  <si>
+    <t>Highly correlated with thtr_days</t>
+  </si>
+  <si>
+    <t>Highly correlated with audience_score</t>
+  </si>
+  <si>
+    <t>Highly correlated with critics_score</t>
+  </si>
+  <si>
+    <t>Highly correlated with genre</t>
+  </si>
+  <si>
+    <t>Not a predictor, but a potential response</t>
+  </si>
+  <si>
+    <t>Log of cast_votes</t>
+  </si>
+  <si>
+    <t>The product of the number of IMDB votes per day and scores</t>
+  </si>
+  <si>
+    <t>Log of votes_per_day_scores</t>
+  </si>
+  <si>
+    <t>Number of days from theatre release date to January 1, 2016</t>
+  </si>
+  <si>
+    <t>The number of IMDB Votes / thtr_days</t>
   </si>
 </sst>
 </file>
@@ -466,9 +490,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,10 +777,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,11 +788,13 @@
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="168.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
         <v>41</v>
@@ -795,7 +824,7 @@
         <v>32</v>
       </c>
       <c r="K1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -824,10 +853,10 @@
         <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -856,10 +885,10 @@
         <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -888,10 +917,10 @@
         <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -920,10 +949,10 @@
         <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -952,10 +981,10 @@
         <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -975,7 +1004,7 @@
         <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -984,10 +1013,10 @@
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K7" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1007,7 +1036,7 @@
         <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8">
         <v>4</v>
@@ -1016,18 +1045,22 @@
         <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K8" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>A8+1</f>
+        <v>1</v>
+      </c>
       <c r="B9" t="s">
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
@@ -1039,19 +1072,19 @@
         <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="K9" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1074,16 +1107,16 @@
         <v>49</v>
       </c>
       <c r="H10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K10" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1106,16 +1139,16 @@
         <v>49</v>
       </c>
       <c r="H11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K11" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1135,19 +1168,19 @@
         <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H12">
         <v>7</v>
       </c>
       <c r="I12" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="K12" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1170,16 +1203,16 @@
         <v>47</v>
       </c>
       <c r="H13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K13" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1199,27 +1232,31 @@
         <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I14" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="J14" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="K14" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>A14+1</f>
+        <v>1</v>
+      </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -1231,19 +1268,19 @@
         <v>36</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J15" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="K15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1263,158 +1300,161 @@
         <v>36</v>
       </c>
       <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
         <v>47</v>
       </c>
-      <c r="H16">
+      <c r="H18">
         <v>1</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I18" t="s">
         <v>0</v>
       </c>
-      <c r="J16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>A16+1</f>
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f>A17+1</f>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18">
-        <v>11</v>
-      </c>
-      <c r="I18" t="s">
-        <v>105</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" ref="A20:A26" si="0">A19+1</f>
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20">
+        <v>13</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f>A18+1</f>
+      <c r="K20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19">
-        <v>12</v>
-      </c>
-      <c r="I19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f>A19+1</f>
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20">
-        <v>8</v>
-      </c>
-      <c r="I20" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f>A20+1</f>
-        <v>5</v>
-      </c>
       <c r="B21" t="s">
         <v>33</v>
       </c>
@@ -1422,101 +1462,101 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J21" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="K21" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23">
+        <v>11</v>
+      </c>
+      <c r="I23" t="s">
+        <v>98</v>
+      </c>
+      <c r="J23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" t="s">
-        <v>68</v>
-      </c>
-      <c r="K22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f>A22+1</f>
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23">
-        <v>3</v>
-      </c>
-      <c r="I23" t="s">
-        <v>2</v>
-      </c>
-      <c r="J23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f>A23+1</f>
-        <v>8</v>
-      </c>
       <c r="B24" t="s">
         <v>33</v>
       </c>
@@ -1533,90 +1573,88 @@
         <v>36</v>
       </c>
       <c r="G24" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H24">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I24" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>A24+1</f>
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26">
         <v>9</v>
       </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F25" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" t="s">
-        <v>48</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J25" t="s">
-        <v>124</v>
-      </c>
-      <c r="K25" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f>A25+1</f>
-        <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26">
-        <v>3</v>
-      </c>
       <c r="I26" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="J26" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1</v>
+        <f>A24+1</f>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
         <v>33</v>
@@ -1625,102 +1663,103 @@
         <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I27" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="K27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>1</v>
+        <f>A26+1</f>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G28" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I28" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="J28" t="s">
-        <v>62</v>
-      </c>
-      <c r="K28" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>A28+1</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
         <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H29">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I29" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="J29" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="K29" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>A29+1</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
@@ -1732,64 +1771,61 @@
         <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F30" t="s">
         <v>37</v>
       </c>
       <c r="G30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H30">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="I30" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="J30" t="s">
-        <v>85</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>A30+1</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31" t="s">
         <v>37</v>
       </c>
       <c r="G31" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I31" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="J31" t="s">
-        <v>95</v>
-      </c>
-      <c r="K31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>A31+1</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -1807,25 +1843,25 @@
         <v>37</v>
       </c>
       <c r="G32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="J32" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="K32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>A30+1</f>
-        <v>4</v>
+        <f>A32+1</f>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
@@ -1843,34 +1879,34 @@
         <v>37</v>
       </c>
       <c r="G33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I33" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="J33" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="K33" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>A32+1</f>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
         <v>44</v>
@@ -1879,22 +1915,25 @@
         <v>37</v>
       </c>
       <c r="G34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="J34" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="K34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>A34+1</f>
-        <v>7</v>
+        <f>A33+1</f>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
@@ -1903,7 +1942,7 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" t="s">
         <v>44</v>
@@ -1915,22 +1954,19 @@
         <v>56</v>
       </c>
       <c r="H35">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="I35" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="J35" t="s">
-        <v>93</v>
-      </c>
-      <c r="K35" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>A35+1</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
         <v>33</v>
@@ -1942,37 +1978,37 @@
         <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G36" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>A34+1</f>
         <v>15</v>
       </c>
-      <c r="I36" t="s">
-        <v>101</v>
-      </c>
-      <c r="J36" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f>A36+1</f>
-        <v>9</v>
-      </c>
       <c r="B37" t="s">
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
         <v>43</v>
@@ -1981,22 +2017,25 @@
         <v>37</v>
       </c>
       <c r="G37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H37">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="K37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>A36+1</f>
-        <v>9</v>
+        <f>A37+1</f>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
         <v>33</v>
@@ -2005,7 +2044,7 @@
         <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E38" t="s">
         <v>44</v>
@@ -2014,25 +2053,22 @@
         <v>37</v>
       </c>
       <c r="G38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="J38" t="s">
-        <v>94</v>
-      </c>
-      <c r="K38" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>A37+1</f>
-        <v>10</v>
+        <f>A38+1</f>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
         <v>33</v>
@@ -2044,28 +2080,28 @@
         <v>33</v>
       </c>
       <c r="E39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F39" t="s">
         <v>37</v>
       </c>
       <c r="G39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="J39" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>A37+1</f>
-        <v>10</v>
+        <f>A39+1</f>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
         <v>33</v>
@@ -2074,34 +2110,31 @@
         <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E40" t="s">
         <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G40" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I40" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="J40" t="s">
-        <v>81</v>
-      </c>
-      <c r="K40" t="s">
-        <v>129</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>A40+1</f>
-        <v>11</v>
+        <f>A39+1</f>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
         <v>33</v>
@@ -2113,31 +2146,31 @@
         <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F41" t="s">
         <v>37</v>
       </c>
       <c r="G41" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I41" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="J41" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="K41" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>A41+1</f>
-        <v>12</v>
+        <f>A40+1</f>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
         <v>33</v>
@@ -2149,73 +2182,73 @@
         <v>33</v>
       </c>
       <c r="E42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F42" t="s">
         <v>37</v>
       </c>
       <c r="G42" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I42" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="J42" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>A41+1</f>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
         <v>33</v>
       </c>
-      <c r="C43" t="s">
-        <v>34</v>
+      <c r="C43" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D43" t="s">
         <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F43" t="s">
         <v>37</v>
       </c>
       <c r="G43" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H43">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="J43" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="K43" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>A42+1</f>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
         <v>33</v>
       </c>
       <c r="C44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E44" t="s">
         <v>44</v>
@@ -2224,31 +2257,34 @@
         <v>37</v>
       </c>
       <c r="G44" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H44">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="J44" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="K44" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f>A44+1</f>
-        <v>14</v>
+        <f>A41+1</f>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
         <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D45" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
         <v>44</v>
@@ -2257,22 +2293,25 @@
         <v>37</v>
       </c>
       <c r="G45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I45" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="J45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="K45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f>A45+1</f>
-        <v>15</v>
+        <f>A42+1</f>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
         <v>33</v>
@@ -2281,7 +2320,7 @@
         <v>33</v>
       </c>
       <c r="D46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E46" t="s">
         <v>44</v>
@@ -2290,22 +2329,19 @@
         <v>37</v>
       </c>
       <c r="G46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H46">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I46" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="J46" t="s">
-        <v>104</v>
-      </c>
-      <c r="K46" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>33</v>
       </c>
@@ -2328,13 +2364,10 @@
         <v>5</v>
       </c>
       <c r="I47" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="J47" t="s">
-        <v>107</v>
-      </c>
-      <c r="K47" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2345,7 +2378,7 @@
         <v>33</v>
       </c>
       <c r="D48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E48" t="s">
         <v>44</v>
@@ -2360,24 +2393,163 @@
         <v>6</v>
       </c>
       <c r="I48" t="s">
+        <v>106</v>
+      </c>
+      <c r="J48" t="s">
+        <v>113</v>
+      </c>
+      <c r="K48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f>A48+1</f>
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" t="s">
+        <v>36</v>
+      </c>
+      <c r="G49" t="s">
+        <v>49</v>
+      </c>
+      <c r="H49">
+        <v>3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" t="s">
+        <v>36</v>
+      </c>
+      <c r="G50" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50" t="s">
+        <v>39</v>
+      </c>
+      <c r="J50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f>A47+1</f>
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" t="s">
+        <v>57</v>
+      </c>
+      <c r="H51">
+        <v>3</v>
+      </c>
+      <c r="I51" t="s">
         <v>114</v>
       </c>
-      <c r="J48" t="s">
-        <v>115</v>
+      <c r="J51" t="s">
+        <v>139</v>
+      </c>
+      <c r="K51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f>A48+1</f>
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" t="s">
+        <v>37</v>
+      </c>
+      <c r="G52" t="s">
+        <v>57</v>
+      </c>
+      <c r="H52">
+        <v>4</v>
+      </c>
+      <c r="I52" t="s">
+        <v>116</v>
+      </c>
+      <c r="J52" t="s">
+        <v>117</v>
+      </c>
+      <c r="K52" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K48">
-    <filterColumn colId="3">
+  <autoFilter ref="A1:K52">
+    <filterColumn colId="4">
       <filters>
-        <filter val="yes"/>
+        <filter val="Derived"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:K48">
-    <sortCondition ref="B2:B48"/>
-    <sortCondition ref="F2:F48"/>
-    <sortCondition ref="I2:I48"/>
+  <sortState ref="A2:K52">
+    <sortCondition ref="B2:B52"/>
+    <sortCondition ref="I2:I52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Last 2 paragraphs then spellcheck
</commit_message>
<xml_diff>
--- a/data/features.xlsx
+++ b/data/features.xlsx
@@ -18,7 +18,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">features!$A$1:$O$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">features!$A$1:$O$71</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1170,10 +1170,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1328,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+1</f>
         <v>2</v>
@@ -1433,7 +1434,7 @@
         <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -1464,7 +1465,7 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6+1</f>
         <v>1</v>
@@ -2013,7 +2014,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="e">
         <f>#REF!+1</f>
         <v>#REF!</v>
@@ -2028,7 +2029,7 @@
         <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" t="s">
         <v>33</v>
@@ -2326,7 +2327,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>A25+1</f>
         <v>1</v>
@@ -2428,7 +2429,7 @@
         <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F28" t="s">
         <v>34</v>
@@ -2470,7 +2471,7 @@
         <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F29" t="s">
         <v>34</v>
@@ -2653,7 +2654,7 @@
         <v>33</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F33" t="s">
         <v>34</v>
@@ -3296,7 +3297,7 @@
         <v>33</v>
       </c>
       <c r="E47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F47" t="s">
         <v>34</v>
@@ -3632,7 +3633,7 @@
         <v>33</v>
       </c>
       <c r="E55" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F55" t="s">
         <v>34</v>
@@ -3674,7 +3675,7 @@
         <v>33</v>
       </c>
       <c r="E56" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F56" t="s">
         <v>34</v>
@@ -3716,7 +3717,7 @@
         <v>33</v>
       </c>
       <c r="E57" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F57" t="s">
         <v>34</v>
@@ -3888,7 +3889,7 @@
         <v>33</v>
       </c>
       <c r="E61" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F61" t="s">
         <v>34</v>
@@ -4162,7 +4163,7 @@
         <v>33</v>
       </c>
       <c r="E67" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F67" t="s">
         <v>33</v>
@@ -4193,7 +4194,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <f>A66+1</f>
         <v>2</v>
@@ -4387,6 +4388,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O71">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="no"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:N52">
     <sortCondition ref="J2:J52"/>
     <sortCondition ref="K2:K52"/>

</xml_diff>